<commit_message>
plc list display and multithrading working
</commit_message>
<xml_diff>
--- a/config/plc_data.xlsx
+++ b/config/plc_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20416"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tamim\PycharmProjects\Project_NODEPORT\config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\001 Cubic\Project_NODEPORT\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D76E82A2-88A5-471B-A310-A3C54D8B66F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9ED2200-8E0E-46F6-8E2E-9CB30083A329}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -49,7 +49,7 @@
     <t>PLC3</t>
   </si>
   <si>
-    <t>192.168.0.130</t>
+    <t>192.168.53.82</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
excel file data appending done
</commit_message>
<xml_diff>
--- a/config/plc_data.xlsx
+++ b/config/plc_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\001 Cubic\Project_NODEPORT\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3C5D6F2-B716-4274-9677-9215F3DBF7A1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E71F79B6-70DD-40A5-B316-A9C8CDEA9815}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>PLC</t>
   </si>
@@ -53,6 +53,9 @@
   </si>
   <si>
     <t>PLC4</t>
+  </si>
+  <si>
+    <t>192.168.96.58</t>
   </si>
 </sst>
 </file>
@@ -418,7 +421,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -500,10 +503,10 @@
         <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C5">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="D5">
         <v>3000</v>

</xml_diff>